<commit_message>
Fix Tx: Add ECH timout
</commit_message>
<xml_diff>
--- a/Electronics/github_public/Rx/BEC/Rx_BEC_V2-1_BOM.xlsx
+++ b/Electronics/github_public/Rx/BEC/Rx_BEC_V2-1_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ludwig\Dropbox\Elektro\GanzeProjekte\eFoil\BREmote\Github\BREmote\Electronics\V2\PCB\Rx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ludwig\Dropbox\Elektro\GanzeProjekte\eFoil\BREmote\Github\BREmote-V2\BREmote-V2\Electronics\github_public\Rx\BEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1336EC4A-E5E2-4E13-A552-6E9DC63DD57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD21E0B-7C2D-4827-A6C4-B8783847FCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3030" windowWidth="17130" windowHeight="13170" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="29100" windowHeight="13170" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Comment</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>C86606</t>
+  </si>
+  <si>
+    <t>C90265, C2977463</t>
   </si>
 </sst>
 </file>
@@ -637,7 +640,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.7109375" defaultRowHeight="15"/>
@@ -737,7 +740,9 @@
         <v>18</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>

</xml_diff>